<commit_message>
Jpetstore Automation testing project
</commit_message>
<xml_diff>
--- a/CapstoneProject/excel_sheet/registration_data.xlsx
+++ b/CapstoneProject/excel_sheet/registration_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wipro\Project\CapstoneProject\excel_sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC41D2A-1D52-437C-BDBC-02A924DC360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AD933B-4217-4BEC-8E96-ECB95608A65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F3584A7F-3D6F-4D04-8BA9-8C52B2EF2167}"/>
   </bookViews>
@@ -105,21 +105,9 @@
     <t>India</t>
   </si>
   <si>
-    <t>pass@123</t>
-  </si>
-  <si>
-    <t>pass2@123</t>
-  </si>
-  <si>
     <t>patil</t>
   </si>
   <si>
-    <t>anand@gmail.com</t>
-  </si>
-  <si>
-    <t>Basu@gmail.com</t>
-  </si>
-  <si>
     <t>2547864865</t>
   </si>
   <si>
@@ -132,13 +120,25 @@
     <t>fdgfdgd</t>
   </si>
   <si>
-    <t>basanagoudpatil123</t>
-  </si>
-  <si>
-    <t>ananthreddi123423</t>
-  </si>
-  <si>
     <t>ananth</t>
+  </si>
+  <si>
+    <t>basanagoudpatilas4573</t>
+  </si>
+  <si>
+    <t>ananthreddithadi563546</t>
+  </si>
+  <si>
+    <t>pass2@1234</t>
+  </si>
+  <si>
+    <t>pass@1234</t>
+  </si>
+  <si>
+    <t>anandpatil@gmail.com</t>
+  </si>
+  <si>
+    <t>Basupatil@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,28 +591,28 @@
     </row>
     <row r="2" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
@@ -638,25 +638,25 @@
     </row>
     <row r="3" spans="1:15" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>7</v>

</xml_diff>